<commit_message>
update and added confluence pdf
</commit_message>
<xml_diff>
--- a/Pomodoro2020.xlsx
+++ b/Pomodoro2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\04_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF9FD44-5744-40EA-BA23-DC9CCF21A31F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFFFEF8-5EAD-4B3B-A2C1-99ECA558094B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="118">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -379,9 +379,6 @@
     <t>planner</t>
   </si>
   <si>
-    <t>cucumber</t>
-  </si>
-  <si>
     <t>cucumber 적용</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
     <t>3GPP 규격 리뷰</t>
   </si>
   <si>
-    <t>C++</t>
-  </si>
-  <si>
     <t>JSON</t>
   </si>
   <si>
@@ -430,9 +424,6 @@
     <t>Agile</t>
   </si>
   <si>
-    <t>Git, Jenkins, GDB</t>
-  </si>
-  <si>
     <t>JIRA, Bamboo CI/CD, Confluence</t>
   </si>
   <si>
@@ -446,6 +437,27 @@
   </si>
   <si>
     <t>book - C++, English, 저장소 정리(google drive, one drive, git, EXT HDD, naver, Local HDD)</t>
+  </si>
+  <si>
+    <t>daily one hour(piano, reading, etc.)</t>
+  </si>
+  <si>
+    <t>Git, Jenkins</t>
+  </si>
+  <si>
+    <t>GDB</t>
+  </si>
+  <si>
+    <t>Cucumber</t>
+  </si>
+  <si>
+    <t>C++, 3GPP TM, Cucumber</t>
+  </si>
+  <si>
+    <t>CPP</t>
+  </si>
+  <si>
+    <t>ENG</t>
   </si>
 </sst>
 </file>
@@ -456,7 +468,7 @@
     <numFmt numFmtId="164" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="165" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +536,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -704,7 +723,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -819,12 +838,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -860,60 +936,6 @@
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1358,8 +1380,8 @@
   <dimension ref="B1:G218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="18" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="18" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1374,197 +1396,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="2:7">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
       <c r="G2" s="37" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="37" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="65" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="56"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="56"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="56"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="60"/>
+      <c r="D10" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="59"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="36"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="62"/>
+      <c r="D14" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="36" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="37" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="37" t="s">
+    <row r="15" spans="2:7">
+      <c r="B15" s="61"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="36" t="s">
+    <row r="16" spans="2:7">
+      <c r="B16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="36" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="36" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="36" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="40"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="36"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="36" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="36" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="22"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1">
@@ -1588,10 +1612,10 @@
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="55">
+      <c r="B19" s="45">
         <v>43962</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="48" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1602,8 +1626,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="56"/>
-      <c r="C20" s="59"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="21" t="s">
         <v>14</v>
       </c>
@@ -1612,8 +1636,8 @@
       <c r="G20" s="24"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="56"/>
-      <c r="C21" s="59"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="21" t="s">
         <v>15</v>
       </c>
@@ -1622,8 +1646,8 @@
       <c r="G21" s="24"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="56"/>
-      <c r="C22" s="59"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="26" t="s">
         <v>7</v>
       </c>
@@ -1632,8 +1656,8 @@
       <c r="G22" s="29"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="56"/>
-      <c r="C23" s="59"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
@@ -1644,8 +1668,8 @@
       <c r="G23" s="20"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="56"/>
-      <c r="C24" s="59"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="2" t="s">
         <v>17</v>
       </c>
@@ -1656,44 +1680,44 @@
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="56"/>
-      <c r="C25" s="59"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="24"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="56"/>
-      <c r="C26" s="59"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="56"/>
-      <c r="C27" s="59"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="57"/>
-      <c r="C28" s="60"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="16" t="s">
         <v>21</v>
       </c>
@@ -1702,10 +1726,10 @@
       <c r="G28" s="19"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="61">
+      <c r="B29" s="39">
         <v>43963</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="42" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="21" t="s">
@@ -1716,28 +1740,32 @@
       <c r="G29" s="24"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="62"/>
-      <c r="C30" s="65"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="43"/>
       <c r="D30" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="F30" s="23"/>
       <c r="G30" s="24"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="62"/>
-      <c r="C31" s="65"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="F31" s="23"/>
       <c r="G31" s="25"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="62"/>
-      <c r="C32" s="65"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="43"/>
       <c r="D32" s="26" t="s">
         <v>7</v>
       </c>
@@ -1746,8 +1774,8 @@
       <c r="G32" s="29"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="62"/>
-      <c r="C33" s="65"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="21" t="s">
         <v>10</v>
       </c>
@@ -1756,48 +1784,56 @@
       <c r="G33" s="24"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="62"/>
-      <c r="C34" s="65"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="43"/>
       <c r="D34" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="22"/>
+      <c r="E34" s="22" t="s">
+        <v>117</v>
+      </c>
       <c r="F34" s="21"/>
       <c r="G34" s="24"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="62"/>
-      <c r="C35" s="65"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="43"/>
       <c r="D35" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="22"/>
+      <c r="E35" s="22" t="s">
+        <v>116</v>
+      </c>
       <c r="F35" s="23"/>
       <c r="G35" s="24"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="62"/>
-      <c r="C36" s="65"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="43"/>
       <c r="D36" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="22"/>
+      <c r="E36" s="22" t="s">
+        <v>116</v>
+      </c>
       <c r="F36" s="21"/>
       <c r="G36" s="24"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="62"/>
-      <c r="C37" s="65"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="E37" s="22"/>
+      <c r="E37" s="22" t="s">
+        <v>116</v>
+      </c>
       <c r="F37" s="23"/>
       <c r="G37" s="24"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="63"/>
-      <c r="C38" s="66"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="44"/>
       <c r="D38" s="16" t="s">
         <v>21</v>
       </c>
@@ -1806,10 +1842,10 @@
       <c r="G38" s="19"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="55">
+      <c r="B39" s="45">
         <v>43964</v>
       </c>
-      <c r="C39" s="58" t="s">
+      <c r="C39" s="48" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -1820,28 +1856,32 @@
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="56"/>
-      <c r="C40" s="59"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="49"/>
       <c r="D40" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="22"/>
+      <c r="E40" s="22" t="s">
+        <v>103</v>
+      </c>
       <c r="F40" s="23"/>
       <c r="G40" s="24"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="56"/>
-      <c r="C41" s="59"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="22"/>
+      <c r="E41" s="22" t="s">
+        <v>103</v>
+      </c>
       <c r="F41" s="23"/>
       <c r="G41" s="24"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="56"/>
-      <c r="C42" s="59"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="26" t="s">
         <v>7</v>
       </c>
@@ -1850,58 +1890,68 @@
       <c r="G42" s="29"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="56"/>
-      <c r="C43" s="59"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="F43" s="7"/>
       <c r="G43" s="20"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="56"/>
-      <c r="C44" s="59"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="F44" s="2"/>
       <c r="G44" s="6"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="56"/>
-      <c r="C45" s="59"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="22"/>
+      <c r="E45" s="22" t="s">
+        <v>114</v>
+      </c>
       <c r="F45" s="21"/>
       <c r="G45" s="24"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="56"/>
-      <c r="C46" s="59"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="22"/>
+      <c r="E46" s="22" t="s">
+        <v>116</v>
+      </c>
       <c r="F46" s="2"/>
       <c r="G46" s="6"/>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="56"/>
-      <c r="C47" s="59"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="49"/>
       <c r="D47" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="22"/>
+      <c r="E47" s="22" t="s">
+        <v>116</v>
+      </c>
       <c r="F47" s="23"/>
       <c r="G47" s="24"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="57"/>
-      <c r="C48" s="60"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="16" t="s">
         <v>21</v>
       </c>
@@ -1910,10 +1960,10 @@
       <c r="G48" s="19"/>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="67">
+      <c r="B49" s="51">
         <v>43965</v>
       </c>
-      <c r="C49" s="64" t="s">
+      <c r="C49" s="42" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="21" t="s">
@@ -1924,8 +1974,8 @@
       <c r="G49" s="24"/>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="68"/>
-      <c r="C50" s="65"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="43"/>
       <c r="D50" s="21" t="s">
         <v>14</v>
       </c>
@@ -1934,8 +1984,8 @@
       <c r="G50" s="24"/>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="68"/>
-      <c r="C51" s="65"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="43"/>
       <c r="D51" s="21" t="s">
         <v>15</v>
       </c>
@@ -1944,8 +1994,8 @@
       <c r="G51" s="25"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="68"/>
-      <c r="C52" s="65"/>
+      <c r="B52" s="52"/>
+      <c r="C52" s="43"/>
       <c r="D52" s="26" t="s">
         <v>7</v>
       </c>
@@ -1954,8 +2004,8 @@
       <c r="G52" s="29"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="68"/>
-      <c r="C53" s="65"/>
+      <c r="B53" s="52"/>
+      <c r="C53" s="43"/>
       <c r="D53" s="21" t="s">
         <v>10</v>
       </c>
@@ -1964,8 +2014,8 @@
       <c r="G53" s="24"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="68"/>
-      <c r="C54" s="65"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="43"/>
       <c r="D54" s="21" t="s">
         <v>82</v>
       </c>
@@ -1974,8 +2024,8 @@
       <c r="G54" s="24"/>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="68"/>
-      <c r="C55" s="65"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="43"/>
       <c r="D55" s="21" t="s">
         <v>83</v>
       </c>
@@ -1984,8 +2034,8 @@
       <c r="G55" s="24"/>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="68"/>
-      <c r="C56" s="65"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="43"/>
       <c r="D56" s="21" t="s">
         <v>84</v>
       </c>
@@ -1994,8 +2044,8 @@
       <c r="G56" s="24"/>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="68"/>
-      <c r="C57" s="65"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="43"/>
       <c r="D57" s="21" t="s">
         <v>85</v>
       </c>
@@ -2004,8 +2054,8 @@
       <c r="G57" s="24"/>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="69"/>
-      <c r="C58" s="66"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="44"/>
       <c r="D58" s="16" t="s">
         <v>21</v>
       </c>
@@ -2014,10 +2064,10 @@
       <c r="G58" s="19"/>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="67">
+      <c r="B59" s="51">
         <v>43966</v>
       </c>
-      <c r="C59" s="58" t="s">
+      <c r="C59" s="48" t="s">
         <v>6</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -2028,8 +2078,8 @@
       <c r="G59" s="6"/>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="68"/>
-      <c r="C60" s="59"/>
+      <c r="B60" s="52"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="21" t="s">
         <v>14</v>
       </c>
@@ -2038,8 +2088,8 @@
       <c r="G60" s="24"/>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="68"/>
-      <c r="C61" s="59"/>
+      <c r="B61" s="52"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="21" t="s">
         <v>15</v>
       </c>
@@ -2048,8 +2098,8 @@
       <c r="G61" s="24"/>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="68"/>
-      <c r="C62" s="59"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="49"/>
       <c r="D62" s="26" t="s">
         <v>7</v>
       </c>
@@ -2058,8 +2108,8 @@
       <c r="G62" s="29"/>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="68"/>
-      <c r="C63" s="59"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="49"/>
       <c r="D63" s="2" t="s">
         <v>16</v>
       </c>
@@ -2068,8 +2118,8 @@
       <c r="G63" s="20"/>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="68"/>
-      <c r="C64" s="59"/>
+      <c r="B64" s="52"/>
+      <c r="C64" s="49"/>
       <c r="D64" s="2" t="s">
         <v>17</v>
       </c>
@@ -2078,8 +2128,8 @@
       <c r="G64" s="6"/>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="68"/>
-      <c r="C65" s="59"/>
+      <c r="B65" s="52"/>
+      <c r="C65" s="49"/>
       <c r="D65" s="21" t="s">
         <v>18</v>
       </c>
@@ -2088,8 +2138,8 @@
       <c r="G65" s="24"/>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="68"/>
-      <c r="C66" s="59"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="49"/>
       <c r="D66" s="2" t="s">
         <v>19</v>
       </c>
@@ -2098,8 +2148,8 @@
       <c r="G66" s="6"/>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="68"/>
-      <c r="C67" s="59"/>
+      <c r="B67" s="52"/>
+      <c r="C67" s="49"/>
       <c r="D67" s="21" t="s">
         <v>20</v>
       </c>
@@ -2108,8 +2158,8 @@
       <c r="G67" s="24"/>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="69"/>
-      <c r="C68" s="60"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="50"/>
       <c r="D68" s="16" t="s">
         <v>21</v>
       </c>
@@ -2118,10 +2168,10 @@
       <c r="G68" s="19"/>
     </row>
     <row r="69" spans="2:7">
-      <c r="B69" s="55">
+      <c r="B69" s="45">
         <v>43969</v>
       </c>
-      <c r="C69" s="58" t="s">
+      <c r="C69" s="48" t="s">
         <v>11</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2132,8 +2182,8 @@
       <c r="G69" s="6"/>
     </row>
     <row r="70" spans="2:7">
-      <c r="B70" s="56"/>
-      <c r="C70" s="59"/>
+      <c r="B70" s="46"/>
+      <c r="C70" s="49"/>
       <c r="D70" s="21" t="s">
         <v>14</v>
       </c>
@@ -2142,8 +2192,8 @@
       <c r="G70" s="24"/>
     </row>
     <row r="71" spans="2:7">
-      <c r="B71" s="56"/>
-      <c r="C71" s="59"/>
+      <c r="B71" s="46"/>
+      <c r="C71" s="49"/>
       <c r="D71" s="21" t="s">
         <v>15</v>
       </c>
@@ -2152,8 +2202,8 @@
       <c r="G71" s="24"/>
     </row>
     <row r="72" spans="2:7">
-      <c r="B72" s="56"/>
-      <c r="C72" s="59"/>
+      <c r="B72" s="46"/>
+      <c r="C72" s="49"/>
       <c r="D72" s="26" t="s">
         <v>7</v>
       </c>
@@ -2162,8 +2212,8 @@
       <c r="G72" s="29"/>
     </row>
     <row r="73" spans="2:7">
-      <c r="B73" s="56"/>
-      <c r="C73" s="59"/>
+      <c r="B73" s="46"/>
+      <c r="C73" s="49"/>
       <c r="D73" s="2" t="s">
         <v>16</v>
       </c>
@@ -2172,8 +2222,8 @@
       <c r="G73" s="20"/>
     </row>
     <row r="74" spans="2:7">
-      <c r="B74" s="56"/>
-      <c r="C74" s="59"/>
+      <c r="B74" s="46"/>
+      <c r="C74" s="49"/>
       <c r="D74" s="2" t="s">
         <v>17</v>
       </c>
@@ -2182,8 +2232,8 @@
       <c r="G74" s="6"/>
     </row>
     <row r="75" spans="2:7">
-      <c r="B75" s="56"/>
-      <c r="C75" s="59"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="49"/>
       <c r="D75" s="21" t="s">
         <v>18</v>
       </c>
@@ -2192,8 +2242,8 @@
       <c r="G75" s="24"/>
     </row>
     <row r="76" spans="2:7">
-      <c r="B76" s="56"/>
-      <c r="C76" s="59"/>
+      <c r="B76" s="46"/>
+      <c r="C76" s="49"/>
       <c r="D76" s="2" t="s">
         <v>19</v>
       </c>
@@ -2202,8 +2252,8 @@
       <c r="G76" s="6"/>
     </row>
     <row r="77" spans="2:7">
-      <c r="B77" s="56"/>
-      <c r="C77" s="59"/>
+      <c r="B77" s="46"/>
+      <c r="C77" s="49"/>
       <c r="D77" s="21" t="s">
         <v>20</v>
       </c>
@@ -2212,8 +2262,8 @@
       <c r="G77" s="24"/>
     </row>
     <row r="78" spans="2:7">
-      <c r="B78" s="57"/>
-      <c r="C78" s="60"/>
+      <c r="B78" s="47"/>
+      <c r="C78" s="50"/>
       <c r="D78" s="16" t="s">
         <v>21</v>
       </c>
@@ -2222,10 +2272,10 @@
       <c r="G78" s="19"/>
     </row>
     <row r="79" spans="2:7">
-      <c r="B79" s="61">
+      <c r="B79" s="39">
         <v>43970</v>
       </c>
-      <c r="C79" s="64" t="s">
+      <c r="C79" s="42" t="s">
         <v>12</v>
       </c>
       <c r="D79" s="21" t="s">
@@ -2236,8 +2286,8 @@
       <c r="G79" s="24"/>
     </row>
     <row r="80" spans="2:7">
-      <c r="B80" s="62"/>
-      <c r="C80" s="65"/>
+      <c r="B80" s="40"/>
+      <c r="C80" s="43"/>
       <c r="D80" s="21" t="s">
         <v>14</v>
       </c>
@@ -2246,8 +2296,8 @@
       <c r="G80" s="24"/>
     </row>
     <row r="81" spans="2:7">
-      <c r="B81" s="62"/>
-      <c r="C81" s="65"/>
+      <c r="B81" s="40"/>
+      <c r="C81" s="43"/>
       <c r="D81" s="21" t="s">
         <v>15</v>
       </c>
@@ -2256,8 +2306,8 @@
       <c r="G81" s="25"/>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="62"/>
-      <c r="C82" s="65"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="43"/>
       <c r="D82" s="26" t="s">
         <v>7</v>
       </c>
@@ -2266,8 +2316,8 @@
       <c r="G82" s="29"/>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="62"/>
-      <c r="C83" s="65"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="43"/>
       <c r="D83" s="21" t="s">
         <v>10</v>
       </c>
@@ -2276,8 +2326,8 @@
       <c r="G83" s="24"/>
     </row>
     <row r="84" spans="2:7">
-      <c r="B84" s="62"/>
-      <c r="C84" s="65"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="43"/>
       <c r="D84" s="21" t="s">
         <v>82</v>
       </c>
@@ -2286,8 +2336,8 @@
       <c r="G84" s="24"/>
     </row>
     <row r="85" spans="2:7">
-      <c r="B85" s="62"/>
-      <c r="C85" s="65"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="43"/>
       <c r="D85" s="21" t="s">
         <v>83</v>
       </c>
@@ -2296,8 +2346,8 @@
       <c r="G85" s="24"/>
     </row>
     <row r="86" spans="2:7">
-      <c r="B86" s="62"/>
-      <c r="C86" s="65"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="43"/>
       <c r="D86" s="21" t="s">
         <v>84</v>
       </c>
@@ -2306,8 +2356,8 @@
       <c r="G86" s="24"/>
     </row>
     <row r="87" spans="2:7">
-      <c r="B87" s="62"/>
-      <c r="C87" s="65"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="43"/>
       <c r="D87" s="21" t="s">
         <v>85</v>
       </c>
@@ -2316,8 +2366,8 @@
       <c r="G87" s="24"/>
     </row>
     <row r="88" spans="2:7">
-      <c r="B88" s="63"/>
-      <c r="C88" s="66"/>
+      <c r="B88" s="41"/>
+      <c r="C88" s="44"/>
       <c r="D88" s="16" t="s">
         <v>21</v>
       </c>
@@ -2326,10 +2376,10 @@
       <c r="G88" s="19"/>
     </row>
     <row r="89" spans="2:7">
-      <c r="B89" s="55">
+      <c r="B89" s="45">
         <v>43971</v>
       </c>
-      <c r="C89" s="58" t="s">
+      <c r="C89" s="48" t="s">
         <v>8</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -2340,8 +2390,8 @@
       <c r="G89" s="6"/>
     </row>
     <row r="90" spans="2:7">
-      <c r="B90" s="56"/>
-      <c r="C90" s="59"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="49"/>
       <c r="D90" s="21" t="s">
         <v>14</v>
       </c>
@@ -2350,8 +2400,8 @@
       <c r="G90" s="24"/>
     </row>
     <row r="91" spans="2:7">
-      <c r="B91" s="56"/>
-      <c r="C91" s="59"/>
+      <c r="B91" s="46"/>
+      <c r="C91" s="49"/>
       <c r="D91" s="21" t="s">
         <v>15</v>
       </c>
@@ -2360,8 +2410,8 @@
       <c r="G91" s="24"/>
     </row>
     <row r="92" spans="2:7">
-      <c r="B92" s="56"/>
-      <c r="C92" s="59"/>
+      <c r="B92" s="46"/>
+      <c r="C92" s="49"/>
       <c r="D92" s="26" t="s">
         <v>7</v>
       </c>
@@ -2370,8 +2420,8 @@
       <c r="G92" s="29"/>
     </row>
     <row r="93" spans="2:7">
-      <c r="B93" s="56"/>
-      <c r="C93" s="59"/>
+      <c r="B93" s="46"/>
+      <c r="C93" s="49"/>
       <c r="D93" s="2" t="s">
         <v>16</v>
       </c>
@@ -2380,8 +2430,8 @@
       <c r="G93" s="20"/>
     </row>
     <row r="94" spans="2:7">
-      <c r="B94" s="56"/>
-      <c r="C94" s="59"/>
+      <c r="B94" s="46"/>
+      <c r="C94" s="49"/>
       <c r="D94" s="2" t="s">
         <v>17</v>
       </c>
@@ -2390,8 +2440,8 @@
       <c r="G94" s="6"/>
     </row>
     <row r="95" spans="2:7">
-      <c r="B95" s="56"/>
-      <c r="C95" s="59"/>
+      <c r="B95" s="46"/>
+      <c r="C95" s="49"/>
       <c r="D95" s="21" t="s">
         <v>18</v>
       </c>
@@ -2400,8 +2450,8 @@
       <c r="G95" s="24"/>
     </row>
     <row r="96" spans="2:7">
-      <c r="B96" s="56"/>
-      <c r="C96" s="59"/>
+      <c r="B96" s="46"/>
+      <c r="C96" s="49"/>
       <c r="D96" s="2" t="s">
         <v>19</v>
       </c>
@@ -2410,8 +2460,8 @@
       <c r="G96" s="6"/>
     </row>
     <row r="97" spans="2:7">
-      <c r="B97" s="56"/>
-      <c r="C97" s="59"/>
+      <c r="B97" s="46"/>
+      <c r="C97" s="49"/>
       <c r="D97" s="21" t="s">
         <v>20</v>
       </c>
@@ -2420,8 +2470,8 @@
       <c r="G97" s="24"/>
     </row>
     <row r="98" spans="2:7">
-      <c r="B98" s="57"/>
-      <c r="C98" s="60"/>
+      <c r="B98" s="47"/>
+      <c r="C98" s="50"/>
       <c r="D98" s="16" t="s">
         <v>21</v>
       </c>
@@ -2430,10 +2480,10 @@
       <c r="G98" s="19"/>
     </row>
     <row r="99" spans="2:7">
-      <c r="B99" s="61">
+      <c r="B99" s="39">
         <v>43972</v>
       </c>
-      <c r="C99" s="64" t="s">
+      <c r="C99" s="42" t="s">
         <v>9</v>
       </c>
       <c r="D99" s="21" t="s">
@@ -2444,8 +2494,8 @@
       <c r="G99" s="24"/>
     </row>
     <row r="100" spans="2:7">
-      <c r="B100" s="62"/>
-      <c r="C100" s="65"/>
+      <c r="B100" s="40"/>
+      <c r="C100" s="43"/>
       <c r="D100" s="21" t="s">
         <v>14</v>
       </c>
@@ -2454,8 +2504,8 @@
       <c r="G100" s="24"/>
     </row>
     <row r="101" spans="2:7">
-      <c r="B101" s="62"/>
-      <c r="C101" s="65"/>
+      <c r="B101" s="40"/>
+      <c r="C101" s="43"/>
       <c r="D101" s="21" t="s">
         <v>15</v>
       </c>
@@ -2464,8 +2514,8 @@
       <c r="G101" s="25"/>
     </row>
     <row r="102" spans="2:7">
-      <c r="B102" s="62"/>
-      <c r="C102" s="65"/>
+      <c r="B102" s="40"/>
+      <c r="C102" s="43"/>
       <c r="D102" s="26" t="s">
         <v>7</v>
       </c>
@@ -2474,8 +2524,8 @@
       <c r="G102" s="29"/>
     </row>
     <row r="103" spans="2:7">
-      <c r="B103" s="62"/>
-      <c r="C103" s="65"/>
+      <c r="B103" s="40"/>
+      <c r="C103" s="43"/>
       <c r="D103" s="21" t="s">
         <v>10</v>
       </c>
@@ -2484,8 +2534,8 @@
       <c r="G103" s="24"/>
     </row>
     <row r="104" spans="2:7">
-      <c r="B104" s="62"/>
-      <c r="C104" s="65"/>
+      <c r="B104" s="40"/>
+      <c r="C104" s="43"/>
       <c r="D104" s="21" t="s">
         <v>82</v>
       </c>
@@ -2494,8 +2544,8 @@
       <c r="G104" s="24"/>
     </row>
     <row r="105" spans="2:7">
-      <c r="B105" s="62"/>
-      <c r="C105" s="65"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="43"/>
       <c r="D105" s="21" t="s">
         <v>83</v>
       </c>
@@ -2504,8 +2554,8 @@
       <c r="G105" s="24"/>
     </row>
     <row r="106" spans="2:7">
-      <c r="B106" s="62"/>
-      <c r="C106" s="65"/>
+      <c r="B106" s="40"/>
+      <c r="C106" s="43"/>
       <c r="D106" s="21" t="s">
         <v>84</v>
       </c>
@@ -2514,8 +2564,8 @@
       <c r="G106" s="24"/>
     </row>
     <row r="107" spans="2:7">
-      <c r="B107" s="62"/>
-      <c r="C107" s="65"/>
+      <c r="B107" s="40"/>
+      <c r="C107" s="43"/>
       <c r="D107" s="21" t="s">
         <v>85</v>
       </c>
@@ -2524,8 +2574,8 @@
       <c r="G107" s="24"/>
     </row>
     <row r="108" spans="2:7">
-      <c r="B108" s="63"/>
-      <c r="C108" s="66"/>
+      <c r="B108" s="41"/>
+      <c r="C108" s="44"/>
       <c r="D108" s="16" t="s">
         <v>21</v>
       </c>
@@ -2534,10 +2584,10 @@
       <c r="G108" s="19"/>
     </row>
     <row r="109" spans="2:7">
-      <c r="B109" s="61">
+      <c r="B109" s="39">
         <v>43973</v>
       </c>
-      <c r="C109" s="64" t="s">
+      <c r="C109" s="42" t="s">
         <v>6</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -2548,8 +2598,8 @@
       <c r="G109" s="6"/>
     </row>
     <row r="110" spans="2:7">
-      <c r="B110" s="62"/>
-      <c r="C110" s="65"/>
+      <c r="B110" s="40"/>
+      <c r="C110" s="43"/>
       <c r="D110" s="21" t="s">
         <v>14</v>
       </c>
@@ -2558,8 +2608,8 @@
       <c r="G110" s="24"/>
     </row>
     <row r="111" spans="2:7">
-      <c r="B111" s="62"/>
-      <c r="C111" s="65"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="43"/>
       <c r="D111" s="21" t="s">
         <v>15</v>
       </c>
@@ -2568,8 +2618,8 @@
       <c r="G111" s="24"/>
     </row>
     <row r="112" spans="2:7">
-      <c r="B112" s="62"/>
-      <c r="C112" s="65"/>
+      <c r="B112" s="40"/>
+      <c r="C112" s="43"/>
       <c r="D112" s="26" t="s">
         <v>7</v>
       </c>
@@ -2578,8 +2628,8 @@
       <c r="G112" s="29"/>
     </row>
     <row r="113" spans="2:7">
-      <c r="B113" s="62"/>
-      <c r="C113" s="65"/>
+      <c r="B113" s="40"/>
+      <c r="C113" s="43"/>
       <c r="D113" s="2" t="s">
         <v>16</v>
       </c>
@@ -2588,8 +2638,8 @@
       <c r="G113" s="20"/>
     </row>
     <row r="114" spans="2:7">
-      <c r="B114" s="62"/>
-      <c r="C114" s="65"/>
+      <c r="B114" s="40"/>
+      <c r="C114" s="43"/>
       <c r="D114" s="2" t="s">
         <v>17</v>
       </c>
@@ -2598,8 +2648,8 @@
       <c r="G114" s="6"/>
     </row>
     <row r="115" spans="2:7">
-      <c r="B115" s="62"/>
-      <c r="C115" s="65"/>
+      <c r="B115" s="40"/>
+      <c r="C115" s="43"/>
       <c r="D115" s="21" t="s">
         <v>18</v>
       </c>
@@ -2608,8 +2658,8 @@
       <c r="G115" s="24"/>
     </row>
     <row r="116" spans="2:7">
-      <c r="B116" s="62"/>
-      <c r="C116" s="65"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="43"/>
       <c r="D116" s="2" t="s">
         <v>19</v>
       </c>
@@ -2618,8 +2668,8 @@
       <c r="G116" s="6"/>
     </row>
     <row r="117" spans="2:7">
-      <c r="B117" s="62"/>
-      <c r="C117" s="65"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="43"/>
       <c r="D117" s="21" t="s">
         <v>20</v>
       </c>
@@ -2628,8 +2678,8 @@
       <c r="G117" s="24"/>
     </row>
     <row r="118" spans="2:7">
-      <c r="B118" s="63"/>
-      <c r="C118" s="66"/>
+      <c r="B118" s="41"/>
+      <c r="C118" s="44"/>
       <c r="D118" s="16" t="s">
         <v>21</v>
       </c>
@@ -2638,10 +2688,10 @@
       <c r="G118" s="19"/>
     </row>
     <row r="119" spans="2:7">
-      <c r="B119" s="55">
+      <c r="B119" s="45">
         <v>43976</v>
       </c>
-      <c r="C119" s="58" t="s">
+      <c r="C119" s="48" t="s">
         <v>11</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -2652,8 +2702,8 @@
       <c r="G119" s="6"/>
     </row>
     <row r="120" spans="2:7">
-      <c r="B120" s="56"/>
-      <c r="C120" s="59"/>
+      <c r="B120" s="46"/>
+      <c r="C120" s="49"/>
       <c r="D120" s="21" t="s">
         <v>14</v>
       </c>
@@ -2662,8 +2712,8 @@
       <c r="G120" s="24"/>
     </row>
     <row r="121" spans="2:7">
-      <c r="B121" s="56"/>
-      <c r="C121" s="59"/>
+      <c r="B121" s="46"/>
+      <c r="C121" s="49"/>
       <c r="D121" s="21" t="s">
         <v>15</v>
       </c>
@@ -2672,8 +2722,8 @@
       <c r="G121" s="24"/>
     </row>
     <row r="122" spans="2:7">
-      <c r="B122" s="56"/>
-      <c r="C122" s="59"/>
+      <c r="B122" s="46"/>
+      <c r="C122" s="49"/>
       <c r="D122" s="26" t="s">
         <v>7</v>
       </c>
@@ -2682,8 +2732,8 @@
       <c r="G122" s="29"/>
     </row>
     <row r="123" spans="2:7">
-      <c r="B123" s="56"/>
-      <c r="C123" s="59"/>
+      <c r="B123" s="46"/>
+      <c r="C123" s="49"/>
       <c r="D123" s="2" t="s">
         <v>16</v>
       </c>
@@ -2692,8 +2742,8 @@
       <c r="G123" s="20"/>
     </row>
     <row r="124" spans="2:7">
-      <c r="B124" s="56"/>
-      <c r="C124" s="59"/>
+      <c r="B124" s="46"/>
+      <c r="C124" s="49"/>
       <c r="D124" s="2" t="s">
         <v>17</v>
       </c>
@@ -2702,8 +2752,8 @@
       <c r="G124" s="6"/>
     </row>
     <row r="125" spans="2:7">
-      <c r="B125" s="56"/>
-      <c r="C125" s="59"/>
+      <c r="B125" s="46"/>
+      <c r="C125" s="49"/>
       <c r="D125" s="21" t="s">
         <v>18</v>
       </c>
@@ -2712,8 +2762,8 @@
       <c r="G125" s="24"/>
     </row>
     <row r="126" spans="2:7">
-      <c r="B126" s="56"/>
-      <c r="C126" s="59"/>
+      <c r="B126" s="46"/>
+      <c r="C126" s="49"/>
       <c r="D126" s="2" t="s">
         <v>19</v>
       </c>
@@ -2722,8 +2772,8 @@
       <c r="G126" s="6"/>
     </row>
     <row r="127" spans="2:7">
-      <c r="B127" s="56"/>
-      <c r="C127" s="59"/>
+      <c r="B127" s="46"/>
+      <c r="C127" s="49"/>
       <c r="D127" s="21" t="s">
         <v>20</v>
       </c>
@@ -2732,8 +2782,8 @@
       <c r="G127" s="24"/>
     </row>
     <row r="128" spans="2:7">
-      <c r="B128" s="57"/>
-      <c r="C128" s="60"/>
+      <c r="B128" s="47"/>
+      <c r="C128" s="50"/>
       <c r="D128" s="16" t="s">
         <v>21</v>
       </c>
@@ -2742,10 +2792,10 @@
       <c r="G128" s="19"/>
     </row>
     <row r="129" spans="2:7">
-      <c r="B129" s="61">
+      <c r="B129" s="39">
         <v>43977</v>
       </c>
-      <c r="C129" s="64" t="s">
+      <c r="C129" s="42" t="s">
         <v>12</v>
       </c>
       <c r="D129" s="21" t="s">
@@ -2756,8 +2806,8 @@
       <c r="G129" s="24"/>
     </row>
     <row r="130" spans="2:7">
-      <c r="B130" s="62"/>
-      <c r="C130" s="65"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="43"/>
       <c r="D130" s="21" t="s">
         <v>14</v>
       </c>
@@ -2766,8 +2816,8 @@
       <c r="G130" s="24"/>
     </row>
     <row r="131" spans="2:7">
-      <c r="B131" s="62"/>
-      <c r="C131" s="65"/>
+      <c r="B131" s="40"/>
+      <c r="C131" s="43"/>
       <c r="D131" s="21" t="s">
         <v>15</v>
       </c>
@@ -2776,8 +2826,8 @@
       <c r="G131" s="25"/>
     </row>
     <row r="132" spans="2:7">
-      <c r="B132" s="62"/>
-      <c r="C132" s="65"/>
+      <c r="B132" s="40"/>
+      <c r="C132" s="43"/>
       <c r="D132" s="26" t="s">
         <v>7</v>
       </c>
@@ -2786,8 +2836,8 @@
       <c r="G132" s="29"/>
     </row>
     <row r="133" spans="2:7">
-      <c r="B133" s="62"/>
-      <c r="C133" s="65"/>
+      <c r="B133" s="40"/>
+      <c r="C133" s="43"/>
       <c r="D133" s="21" t="s">
         <v>10</v>
       </c>
@@ -2796,8 +2846,8 @@
       <c r="G133" s="24"/>
     </row>
     <row r="134" spans="2:7">
-      <c r="B134" s="62"/>
-      <c r="C134" s="65"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="43"/>
       <c r="D134" s="21" t="s">
         <v>82</v>
       </c>
@@ -2806,8 +2856,8 @@
       <c r="G134" s="24"/>
     </row>
     <row r="135" spans="2:7">
-      <c r="B135" s="62"/>
-      <c r="C135" s="65"/>
+      <c r="B135" s="40"/>
+      <c r="C135" s="43"/>
       <c r="D135" s="21" t="s">
         <v>83</v>
       </c>
@@ -2816,8 +2866,8 @@
       <c r="G135" s="24"/>
     </row>
     <row r="136" spans="2:7">
-      <c r="B136" s="62"/>
-      <c r="C136" s="65"/>
+      <c r="B136" s="40"/>
+      <c r="C136" s="43"/>
       <c r="D136" s="21" t="s">
         <v>84</v>
       </c>
@@ -2826,8 +2876,8 @@
       <c r="G136" s="24"/>
     </row>
     <row r="137" spans="2:7">
-      <c r="B137" s="62"/>
-      <c r="C137" s="65"/>
+      <c r="B137" s="40"/>
+      <c r="C137" s="43"/>
       <c r="D137" s="21" t="s">
         <v>85</v>
       </c>
@@ -2836,8 +2886,8 @@
       <c r="G137" s="24"/>
     </row>
     <row r="138" spans="2:7">
-      <c r="B138" s="63"/>
-      <c r="C138" s="66"/>
+      <c r="B138" s="41"/>
+      <c r="C138" s="44"/>
       <c r="D138" s="16" t="s">
         <v>21</v>
       </c>
@@ -2846,10 +2896,10 @@
       <c r="G138" s="19"/>
     </row>
     <row r="139" spans="2:7">
-      <c r="B139" s="55">
+      <c r="B139" s="45">
         <v>43978</v>
       </c>
-      <c r="C139" s="58" t="s">
+      <c r="C139" s="48" t="s">
         <v>8</v>
       </c>
       <c r="D139" s="2" t="s">
@@ -2860,8 +2910,8 @@
       <c r="G139" s="6"/>
     </row>
     <row r="140" spans="2:7">
-      <c r="B140" s="56"/>
-      <c r="C140" s="59"/>
+      <c r="B140" s="46"/>
+      <c r="C140" s="49"/>
       <c r="D140" s="21" t="s">
         <v>14</v>
       </c>
@@ -2870,8 +2920,8 @@
       <c r="G140" s="24"/>
     </row>
     <row r="141" spans="2:7">
-      <c r="B141" s="56"/>
-      <c r="C141" s="59"/>
+      <c r="B141" s="46"/>
+      <c r="C141" s="49"/>
       <c r="D141" s="21" t="s">
         <v>15</v>
       </c>
@@ -2880,8 +2930,8 @@
       <c r="G141" s="24"/>
     </row>
     <row r="142" spans="2:7">
-      <c r="B142" s="56"/>
-      <c r="C142" s="59"/>
+      <c r="B142" s="46"/>
+      <c r="C142" s="49"/>
       <c r="D142" s="26" t="s">
         <v>7</v>
       </c>
@@ -2890,8 +2940,8 @@
       <c r="G142" s="29"/>
     </row>
     <row r="143" spans="2:7">
-      <c r="B143" s="56"/>
-      <c r="C143" s="59"/>
+      <c r="B143" s="46"/>
+      <c r="C143" s="49"/>
       <c r="D143" s="2" t="s">
         <v>16</v>
       </c>
@@ -2900,8 +2950,8 @@
       <c r="G143" s="20"/>
     </row>
     <row r="144" spans="2:7">
-      <c r="B144" s="56"/>
-      <c r="C144" s="59"/>
+      <c r="B144" s="46"/>
+      <c r="C144" s="49"/>
       <c r="D144" s="2" t="s">
         <v>17</v>
       </c>
@@ -2910,8 +2960,8 @@
       <c r="G144" s="6"/>
     </row>
     <row r="145" spans="2:7">
-      <c r="B145" s="56"/>
-      <c r="C145" s="59"/>
+      <c r="B145" s="46"/>
+      <c r="C145" s="49"/>
       <c r="D145" s="21" t="s">
         <v>18</v>
       </c>
@@ -2920,8 +2970,8 @@
       <c r="G145" s="24"/>
     </row>
     <row r="146" spans="2:7">
-      <c r="B146" s="56"/>
-      <c r="C146" s="59"/>
+      <c r="B146" s="46"/>
+      <c r="C146" s="49"/>
       <c r="D146" s="2" t="s">
         <v>19</v>
       </c>
@@ -2930,8 +2980,8 @@
       <c r="G146" s="6"/>
     </row>
     <row r="147" spans="2:7">
-      <c r="B147" s="56"/>
-      <c r="C147" s="59"/>
+      <c r="B147" s="46"/>
+      <c r="C147" s="49"/>
       <c r="D147" s="21" t="s">
         <v>20</v>
       </c>
@@ -2940,8 +2990,8 @@
       <c r="G147" s="24"/>
     </row>
     <row r="148" spans="2:7">
-      <c r="B148" s="57"/>
-      <c r="C148" s="60"/>
+      <c r="B148" s="47"/>
+      <c r="C148" s="50"/>
       <c r="D148" s="16" t="s">
         <v>21</v>
       </c>
@@ -2950,10 +3000,10 @@
       <c r="G148" s="19"/>
     </row>
     <row r="149" spans="2:7">
-      <c r="B149" s="61">
+      <c r="B149" s="39">
         <v>43979</v>
       </c>
-      <c r="C149" s="64" t="s">
+      <c r="C149" s="42" t="s">
         <v>9</v>
       </c>
       <c r="D149" s="21" t="s">
@@ -2964,8 +3014,8 @@
       <c r="G149" s="24"/>
     </row>
     <row r="150" spans="2:7">
-      <c r="B150" s="62"/>
-      <c r="C150" s="65"/>
+      <c r="B150" s="40"/>
+      <c r="C150" s="43"/>
       <c r="D150" s="21" t="s">
         <v>14</v>
       </c>
@@ -2974,8 +3024,8 @@
       <c r="G150" s="24"/>
     </row>
     <row r="151" spans="2:7">
-      <c r="B151" s="62"/>
-      <c r="C151" s="65"/>
+      <c r="B151" s="40"/>
+      <c r="C151" s="43"/>
       <c r="D151" s="21" t="s">
         <v>15</v>
       </c>
@@ -2984,8 +3034,8 @@
       <c r="G151" s="25"/>
     </row>
     <row r="152" spans="2:7">
-      <c r="B152" s="62"/>
-      <c r="C152" s="65"/>
+      <c r="B152" s="40"/>
+      <c r="C152" s="43"/>
       <c r="D152" s="26" t="s">
         <v>7</v>
       </c>
@@ -2994,8 +3044,8 @@
       <c r="G152" s="29"/>
     </row>
     <row r="153" spans="2:7">
-      <c r="B153" s="62"/>
-      <c r="C153" s="65"/>
+      <c r="B153" s="40"/>
+      <c r="C153" s="43"/>
       <c r="D153" s="21" t="s">
         <v>10</v>
       </c>
@@ -3004,8 +3054,8 @@
       <c r="G153" s="24"/>
     </row>
     <row r="154" spans="2:7">
-      <c r="B154" s="62"/>
-      <c r="C154" s="65"/>
+      <c r="B154" s="40"/>
+      <c r="C154" s="43"/>
       <c r="D154" s="21" t="s">
         <v>82</v>
       </c>
@@ -3014,8 +3064,8 @@
       <c r="G154" s="24"/>
     </row>
     <row r="155" spans="2:7">
-      <c r="B155" s="62"/>
-      <c r="C155" s="65"/>
+      <c r="B155" s="40"/>
+      <c r="C155" s="43"/>
       <c r="D155" s="21" t="s">
         <v>83</v>
       </c>
@@ -3024,8 +3074,8 @@
       <c r="G155" s="24"/>
     </row>
     <row r="156" spans="2:7">
-      <c r="B156" s="62"/>
-      <c r="C156" s="65"/>
+      <c r="B156" s="40"/>
+      <c r="C156" s="43"/>
       <c r="D156" s="21" t="s">
         <v>84</v>
       </c>
@@ -3034,8 +3084,8 @@
       <c r="G156" s="24"/>
     </row>
     <row r="157" spans="2:7">
-      <c r="B157" s="62"/>
-      <c r="C157" s="65"/>
+      <c r="B157" s="40"/>
+      <c r="C157" s="43"/>
       <c r="D157" s="21" t="s">
         <v>85</v>
       </c>
@@ -3044,8 +3094,8 @@
       <c r="G157" s="24"/>
     </row>
     <row r="158" spans="2:7">
-      <c r="B158" s="63"/>
-      <c r="C158" s="66"/>
+      <c r="B158" s="41"/>
+      <c r="C158" s="44"/>
       <c r="D158" s="16" t="s">
         <v>21</v>
       </c>
@@ -3054,10 +3104,10 @@
       <c r="G158" s="19"/>
     </row>
     <row r="159" spans="2:7">
-      <c r="B159" s="61">
+      <c r="B159" s="39">
         <v>43980</v>
       </c>
-      <c r="C159" s="64" t="s">
+      <c r="C159" s="42" t="s">
         <v>6</v>
       </c>
       <c r="D159" s="2" t="s">
@@ -3068,8 +3118,8 @@
       <c r="G159" s="6"/>
     </row>
     <row r="160" spans="2:7">
-      <c r="B160" s="62"/>
-      <c r="C160" s="65"/>
+      <c r="B160" s="40"/>
+      <c r="C160" s="43"/>
       <c r="D160" s="21" t="s">
         <v>14</v>
       </c>
@@ -3078,8 +3128,8 @@
       <c r="G160" s="24"/>
     </row>
     <row r="161" spans="2:7">
-      <c r="B161" s="62"/>
-      <c r="C161" s="65"/>
+      <c r="B161" s="40"/>
+      <c r="C161" s="43"/>
       <c r="D161" s="21" t="s">
         <v>15</v>
       </c>
@@ -3088,8 +3138,8 @@
       <c r="G161" s="24"/>
     </row>
     <row r="162" spans="2:7">
-      <c r="B162" s="62"/>
-      <c r="C162" s="65"/>
+      <c r="B162" s="40"/>
+      <c r="C162" s="43"/>
       <c r="D162" s="26" t="s">
         <v>7</v>
       </c>
@@ -3098,8 +3148,8 @@
       <c r="G162" s="29"/>
     </row>
     <row r="163" spans="2:7">
-      <c r="B163" s="62"/>
-      <c r="C163" s="65"/>
+      <c r="B163" s="40"/>
+      <c r="C163" s="43"/>
       <c r="D163" s="2" t="s">
         <v>16</v>
       </c>
@@ -3108,8 +3158,8 @@
       <c r="G163" s="20"/>
     </row>
     <row r="164" spans="2:7">
-      <c r="B164" s="62"/>
-      <c r="C164" s="65"/>
+      <c r="B164" s="40"/>
+      <c r="C164" s="43"/>
       <c r="D164" s="2" t="s">
         <v>17</v>
       </c>
@@ -3118,8 +3168,8 @@
       <c r="G164" s="6"/>
     </row>
     <row r="165" spans="2:7">
-      <c r="B165" s="62"/>
-      <c r="C165" s="65"/>
+      <c r="B165" s="40"/>
+      <c r="C165" s="43"/>
       <c r="D165" s="21" t="s">
         <v>18</v>
       </c>
@@ -3128,8 +3178,8 @@
       <c r="G165" s="24"/>
     </row>
     <row r="166" spans="2:7">
-      <c r="B166" s="62"/>
-      <c r="C166" s="65"/>
+      <c r="B166" s="40"/>
+      <c r="C166" s="43"/>
       <c r="D166" s="2" t="s">
         <v>19</v>
       </c>
@@ -3138,8 +3188,8 @@
       <c r="G166" s="6"/>
     </row>
     <row r="167" spans="2:7">
-      <c r="B167" s="62"/>
-      <c r="C167" s="65"/>
+      <c r="B167" s="40"/>
+      <c r="C167" s="43"/>
       <c r="D167" s="21" t="s">
         <v>20</v>
       </c>
@@ -3148,8 +3198,8 @@
       <c r="G167" s="24"/>
     </row>
     <row r="168" spans="2:7">
-      <c r="B168" s="63"/>
-      <c r="C168" s="66"/>
+      <c r="B168" s="41"/>
+      <c r="C168" s="44"/>
       <c r="D168" s="16" t="s">
         <v>21</v>
       </c>
@@ -3158,8 +3208,8 @@
       <c r="G168" s="19"/>
     </row>
     <row r="169" spans="2:7">
-      <c r="B169" s="55"/>
-      <c r="C169" s="58" t="s">
+      <c r="B169" s="45"/>
+      <c r="C169" s="48" t="s">
         <v>77</v>
       </c>
       <c r="D169" s="2" t="s">
@@ -3170,8 +3220,8 @@
       <c r="G169" s="6"/>
     </row>
     <row r="170" spans="2:7">
-      <c r="B170" s="56"/>
-      <c r="C170" s="59"/>
+      <c r="B170" s="46"/>
+      <c r="C170" s="49"/>
       <c r="D170" s="21" t="s">
         <v>14</v>
       </c>
@@ -3180,8 +3230,8 @@
       <c r="G170" s="24"/>
     </row>
     <row r="171" spans="2:7">
-      <c r="B171" s="56"/>
-      <c r="C171" s="59"/>
+      <c r="B171" s="46"/>
+      <c r="C171" s="49"/>
       <c r="D171" s="21" t="s">
         <v>15</v>
       </c>
@@ -3190,8 +3240,8 @@
       <c r="G171" s="24"/>
     </row>
     <row r="172" spans="2:7">
-      <c r="B172" s="56"/>
-      <c r="C172" s="59"/>
+      <c r="B172" s="46"/>
+      <c r="C172" s="49"/>
       <c r="D172" s="26" t="s">
         <v>7</v>
       </c>
@@ -3200,8 +3250,8 @@
       <c r="G172" s="29"/>
     </row>
     <row r="173" spans="2:7">
-      <c r="B173" s="56"/>
-      <c r="C173" s="59"/>
+      <c r="B173" s="46"/>
+      <c r="C173" s="49"/>
       <c r="D173" s="2" t="s">
         <v>16</v>
       </c>
@@ -3210,8 +3260,8 @@
       <c r="G173" s="20"/>
     </row>
     <row r="174" spans="2:7">
-      <c r="B174" s="56"/>
-      <c r="C174" s="59"/>
+      <c r="B174" s="46"/>
+      <c r="C174" s="49"/>
       <c r="D174" s="2" t="s">
         <v>17</v>
       </c>
@@ -3220,8 +3270,8 @@
       <c r="G174" s="6"/>
     </row>
     <row r="175" spans="2:7">
-      <c r="B175" s="56"/>
-      <c r="C175" s="59"/>
+      <c r="B175" s="46"/>
+      <c r="C175" s="49"/>
       <c r="D175" s="21" t="s">
         <v>18</v>
       </c>
@@ -3230,8 +3280,8 @@
       <c r="G175" s="24"/>
     </row>
     <row r="176" spans="2:7">
-      <c r="B176" s="56"/>
-      <c r="C176" s="59"/>
+      <c r="B176" s="46"/>
+      <c r="C176" s="49"/>
       <c r="D176" s="2" t="s">
         <v>19</v>
       </c>
@@ -3240,8 +3290,8 @@
       <c r="G176" s="6"/>
     </row>
     <row r="177" spans="2:7">
-      <c r="B177" s="56"/>
-      <c r="C177" s="59"/>
+      <c r="B177" s="46"/>
+      <c r="C177" s="49"/>
       <c r="D177" s="21" t="s">
         <v>20</v>
       </c>
@@ -3250,8 +3300,8 @@
       <c r="G177" s="24"/>
     </row>
     <row r="178" spans="2:7">
-      <c r="B178" s="57"/>
-      <c r="C178" s="60"/>
+      <c r="B178" s="47"/>
+      <c r="C178" s="50"/>
       <c r="D178" s="16" t="s">
         <v>21</v>
       </c>
@@ -3260,8 +3310,8 @@
       <c r="G178" s="19"/>
     </row>
     <row r="179" spans="2:7">
-      <c r="B179" s="61"/>
-      <c r="C179" s="64" t="s">
+      <c r="B179" s="39"/>
+      <c r="C179" s="42" t="s">
         <v>78</v>
       </c>
       <c r="D179" s="21" t="s">
@@ -3272,8 +3322,8 @@
       <c r="G179" s="24"/>
     </row>
     <row r="180" spans="2:7">
-      <c r="B180" s="62"/>
-      <c r="C180" s="65"/>
+      <c r="B180" s="40"/>
+      <c r="C180" s="43"/>
       <c r="D180" s="21" t="s">
         <v>14</v>
       </c>
@@ -3282,8 +3332,8 @@
       <c r="G180" s="24"/>
     </row>
     <row r="181" spans="2:7">
-      <c r="B181" s="62"/>
-      <c r="C181" s="65"/>
+      <c r="B181" s="40"/>
+      <c r="C181" s="43"/>
       <c r="D181" s="21" t="s">
         <v>15</v>
       </c>
@@ -3292,8 +3342,8 @@
       <c r="G181" s="25"/>
     </row>
     <row r="182" spans="2:7">
-      <c r="B182" s="62"/>
-      <c r="C182" s="65"/>
+      <c r="B182" s="40"/>
+      <c r="C182" s="43"/>
       <c r="D182" s="26" t="s">
         <v>7</v>
       </c>
@@ -3302,8 +3352,8 @@
       <c r="G182" s="29"/>
     </row>
     <row r="183" spans="2:7">
-      <c r="B183" s="62"/>
-      <c r="C183" s="65"/>
+      <c r="B183" s="40"/>
+      <c r="C183" s="43"/>
       <c r="D183" s="21" t="s">
         <v>10</v>
       </c>
@@ -3312,8 +3362,8 @@
       <c r="G183" s="24"/>
     </row>
     <row r="184" spans="2:7">
-      <c r="B184" s="62"/>
-      <c r="C184" s="65"/>
+      <c r="B184" s="40"/>
+      <c r="C184" s="43"/>
       <c r="D184" s="21" t="s">
         <v>82</v>
       </c>
@@ -3322,8 +3372,8 @@
       <c r="G184" s="24"/>
     </row>
     <row r="185" spans="2:7">
-      <c r="B185" s="62"/>
-      <c r="C185" s="65"/>
+      <c r="B185" s="40"/>
+      <c r="C185" s="43"/>
       <c r="D185" s="21" t="s">
         <v>83</v>
       </c>
@@ -3332,8 +3382,8 @@
       <c r="G185" s="24"/>
     </row>
     <row r="186" spans="2:7">
-      <c r="B186" s="62"/>
-      <c r="C186" s="65"/>
+      <c r="B186" s="40"/>
+      <c r="C186" s="43"/>
       <c r="D186" s="21" t="s">
         <v>84</v>
       </c>
@@ -3342,8 +3392,8 @@
       <c r="G186" s="24"/>
     </row>
     <row r="187" spans="2:7">
-      <c r="B187" s="62"/>
-      <c r="C187" s="65"/>
+      <c r="B187" s="40"/>
+      <c r="C187" s="43"/>
       <c r="D187" s="21" t="s">
         <v>85</v>
       </c>
@@ -3352,8 +3402,8 @@
       <c r="G187" s="24"/>
     </row>
     <row r="188" spans="2:7">
-      <c r="B188" s="63"/>
-      <c r="C188" s="66"/>
+      <c r="B188" s="41"/>
+      <c r="C188" s="44"/>
       <c r="D188" s="16" t="s">
         <v>21</v>
       </c>
@@ -3362,8 +3412,8 @@
       <c r="G188" s="19"/>
     </row>
     <row r="189" spans="2:7">
-      <c r="B189" s="55"/>
-      <c r="C189" s="58" t="s">
+      <c r="B189" s="45"/>
+      <c r="C189" s="48" t="s">
         <v>79</v>
       </c>
       <c r="D189" s="2" t="s">
@@ -3374,8 +3424,8 @@
       <c r="G189" s="6"/>
     </row>
     <row r="190" spans="2:7">
-      <c r="B190" s="56"/>
-      <c r="C190" s="59"/>
+      <c r="B190" s="46"/>
+      <c r="C190" s="49"/>
       <c r="D190" s="21" t="s">
         <v>14</v>
       </c>
@@ -3384,8 +3434,8 @@
       <c r="G190" s="24"/>
     </row>
     <row r="191" spans="2:7">
-      <c r="B191" s="56"/>
-      <c r="C191" s="59"/>
+      <c r="B191" s="46"/>
+      <c r="C191" s="49"/>
       <c r="D191" s="21" t="s">
         <v>15</v>
       </c>
@@ -3394,8 +3444,8 @@
       <c r="G191" s="24"/>
     </row>
     <row r="192" spans="2:7">
-      <c r="B192" s="56"/>
-      <c r="C192" s="59"/>
+      <c r="B192" s="46"/>
+      <c r="C192" s="49"/>
       <c r="D192" s="26" t="s">
         <v>7</v>
       </c>
@@ -3404,8 +3454,8 @@
       <c r="G192" s="29"/>
     </row>
     <row r="193" spans="2:7">
-      <c r="B193" s="56"/>
-      <c r="C193" s="59"/>
+      <c r="B193" s="46"/>
+      <c r="C193" s="49"/>
       <c r="D193" s="2" t="s">
         <v>16</v>
       </c>
@@ -3414,8 +3464,8 @@
       <c r="G193" s="20"/>
     </row>
     <row r="194" spans="2:7">
-      <c r="B194" s="56"/>
-      <c r="C194" s="59"/>
+      <c r="B194" s="46"/>
+      <c r="C194" s="49"/>
       <c r="D194" s="2" t="s">
         <v>17</v>
       </c>
@@ -3424,8 +3474,8 @@
       <c r="G194" s="6"/>
     </row>
     <row r="195" spans="2:7">
-      <c r="B195" s="56"/>
-      <c r="C195" s="59"/>
+      <c r="B195" s="46"/>
+      <c r="C195" s="49"/>
       <c r="D195" s="21" t="s">
         <v>18</v>
       </c>
@@ -3434,8 +3484,8 @@
       <c r="G195" s="24"/>
     </row>
     <row r="196" spans="2:7">
-      <c r="B196" s="56"/>
-      <c r="C196" s="59"/>
+      <c r="B196" s="46"/>
+      <c r="C196" s="49"/>
       <c r="D196" s="2" t="s">
         <v>19</v>
       </c>
@@ -3444,8 +3494,8 @@
       <c r="G196" s="6"/>
     </row>
     <row r="197" spans="2:7">
-      <c r="B197" s="56"/>
-      <c r="C197" s="59"/>
+      <c r="B197" s="46"/>
+      <c r="C197" s="49"/>
       <c r="D197" s="21" t="s">
         <v>20</v>
       </c>
@@ -3454,8 +3504,8 @@
       <c r="G197" s="24"/>
     </row>
     <row r="198" spans="2:7">
-      <c r="B198" s="57"/>
-      <c r="C198" s="60"/>
+      <c r="B198" s="47"/>
+      <c r="C198" s="50"/>
       <c r="D198" s="16" t="s">
         <v>21</v>
       </c>
@@ -3464,8 +3514,8 @@
       <c r="G198" s="19"/>
     </row>
     <row r="199" spans="2:7">
-      <c r="B199" s="61"/>
-      <c r="C199" s="64" t="s">
+      <c r="B199" s="39"/>
+      <c r="C199" s="42" t="s">
         <v>80</v>
       </c>
       <c r="D199" s="21" t="s">
@@ -3476,8 +3526,8 @@
       <c r="G199" s="24"/>
     </row>
     <row r="200" spans="2:7">
-      <c r="B200" s="62"/>
-      <c r="C200" s="65"/>
+      <c r="B200" s="40"/>
+      <c r="C200" s="43"/>
       <c r="D200" s="21" t="s">
         <v>14</v>
       </c>
@@ -3486,8 +3536,8 @@
       <c r="G200" s="24"/>
     </row>
     <row r="201" spans="2:7">
-      <c r="B201" s="62"/>
-      <c r="C201" s="65"/>
+      <c r="B201" s="40"/>
+      <c r="C201" s="43"/>
       <c r="D201" s="21" t="s">
         <v>15</v>
       </c>
@@ -3496,8 +3546,8 @@
       <c r="G201" s="25"/>
     </row>
     <row r="202" spans="2:7">
-      <c r="B202" s="62"/>
-      <c r="C202" s="65"/>
+      <c r="B202" s="40"/>
+      <c r="C202" s="43"/>
       <c r="D202" s="26" t="s">
         <v>7</v>
       </c>
@@ -3506,8 +3556,8 @@
       <c r="G202" s="29"/>
     </row>
     <row r="203" spans="2:7">
-      <c r="B203" s="62"/>
-      <c r="C203" s="65"/>
+      <c r="B203" s="40"/>
+      <c r="C203" s="43"/>
       <c r="D203" s="21" t="s">
         <v>10</v>
       </c>
@@ -3516,8 +3566,8 @@
       <c r="G203" s="24"/>
     </row>
     <row r="204" spans="2:7">
-      <c r="B204" s="62"/>
-      <c r="C204" s="65"/>
+      <c r="B204" s="40"/>
+      <c r="C204" s="43"/>
       <c r="D204" s="21" t="s">
         <v>82</v>
       </c>
@@ -3526,8 +3576,8 @@
       <c r="G204" s="24"/>
     </row>
     <row r="205" spans="2:7">
-      <c r="B205" s="62"/>
-      <c r="C205" s="65"/>
+      <c r="B205" s="40"/>
+      <c r="C205" s="43"/>
       <c r="D205" s="21" t="s">
         <v>83</v>
       </c>
@@ -3536,8 +3586,8 @@
       <c r="G205" s="24"/>
     </row>
     <row r="206" spans="2:7">
-      <c r="B206" s="62"/>
-      <c r="C206" s="65"/>
+      <c r="B206" s="40"/>
+      <c r="C206" s="43"/>
       <c r="D206" s="21" t="s">
         <v>84</v>
       </c>
@@ -3546,8 +3596,8 @@
       <c r="G206" s="24"/>
     </row>
     <row r="207" spans="2:7">
-      <c r="B207" s="62"/>
-      <c r="C207" s="65"/>
+      <c r="B207" s="40"/>
+      <c r="C207" s="43"/>
       <c r="D207" s="21" t="s">
         <v>85</v>
       </c>
@@ -3556,8 +3606,8 @@
       <c r="G207" s="24"/>
     </row>
     <row r="208" spans="2:7">
-      <c r="B208" s="63"/>
-      <c r="C208" s="66"/>
+      <c r="B208" s="41"/>
+      <c r="C208" s="44"/>
       <c r="D208" s="16" t="s">
         <v>21</v>
       </c>
@@ -3566,8 +3616,8 @@
       <c r="G208" s="19"/>
     </row>
     <row r="209" spans="2:7">
-      <c r="B209" s="61"/>
-      <c r="C209" s="64" t="s">
+      <c r="B209" s="39"/>
+      <c r="C209" s="42" t="s">
         <v>81</v>
       </c>
       <c r="D209" s="2" t="s">
@@ -3578,8 +3628,8 @@
       <c r="G209" s="6"/>
     </row>
     <row r="210" spans="2:7">
-      <c r="B210" s="62"/>
-      <c r="C210" s="65"/>
+      <c r="B210" s="40"/>
+      <c r="C210" s="43"/>
       <c r="D210" s="21" t="s">
         <v>14</v>
       </c>
@@ -3588,8 +3638,8 @@
       <c r="G210" s="24"/>
     </row>
     <row r="211" spans="2:7">
-      <c r="B211" s="62"/>
-      <c r="C211" s="65"/>
+      <c r="B211" s="40"/>
+      <c r="C211" s="43"/>
       <c r="D211" s="21" t="s">
         <v>15</v>
       </c>
@@ -3598,8 +3648,8 @@
       <c r="G211" s="24"/>
     </row>
     <row r="212" spans="2:7">
-      <c r="B212" s="62"/>
-      <c r="C212" s="65"/>
+      <c r="B212" s="40"/>
+      <c r="C212" s="43"/>
       <c r="D212" s="26" t="s">
         <v>7</v>
       </c>
@@ -3608,8 +3658,8 @@
       <c r="G212" s="29"/>
     </row>
     <row r="213" spans="2:7">
-      <c r="B213" s="62"/>
-      <c r="C213" s="65"/>
+      <c r="B213" s="40"/>
+      <c r="C213" s="43"/>
       <c r="D213" s="2" t="s">
         <v>16</v>
       </c>
@@ -3618,8 +3668,8 @@
       <c r="G213" s="20"/>
     </row>
     <row r="214" spans="2:7">
-      <c r="B214" s="62"/>
-      <c r="C214" s="65"/>
+      <c r="B214" s="40"/>
+      <c r="C214" s="43"/>
       <c r="D214" s="2" t="s">
         <v>17</v>
       </c>
@@ -3628,8 +3678,8 @@
       <c r="G214" s="6"/>
     </row>
     <row r="215" spans="2:7">
-      <c r="B215" s="62"/>
-      <c r="C215" s="65"/>
+      <c r="B215" s="40"/>
+      <c r="C215" s="43"/>
       <c r="D215" s="21" t="s">
         <v>18</v>
       </c>
@@ -3638,8 +3688,8 @@
       <c r="G215" s="24"/>
     </row>
     <row r="216" spans="2:7">
-      <c r="B216" s="62"/>
-      <c r="C216" s="65"/>
+      <c r="B216" s="40"/>
+      <c r="C216" s="43"/>
       <c r="D216" s="2" t="s">
         <v>19</v>
       </c>
@@ -3648,8 +3698,8 @@
       <c r="G216" s="6"/>
     </row>
     <row r="217" spans="2:7">
-      <c r="B217" s="62"/>
-      <c r="C217" s="65"/>
+      <c r="B217" s="40"/>
+      <c r="C217" s="43"/>
       <c r="D217" s="21" t="s">
         <v>20</v>
       </c>
@@ -3658,8 +3708,8 @@
       <c r="G217" s="24"/>
     </row>
     <row r="218" spans="2:7">
-      <c r="B218" s="63"/>
-      <c r="C218" s="66"/>
+      <c r="B218" s="41"/>
+      <c r="C218" s="44"/>
       <c r="D218" s="16" t="s">
         <v>21</v>
       </c>
@@ -3669,46 +3719,11 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="B199:B208"/>
-    <mergeCell ref="C199:C208"/>
-    <mergeCell ref="B209:B218"/>
-    <mergeCell ref="C209:C218"/>
-    <mergeCell ref="B169:B178"/>
-    <mergeCell ref="C169:C178"/>
-    <mergeCell ref="B179:B188"/>
-    <mergeCell ref="C179:C188"/>
-    <mergeCell ref="B189:B198"/>
-    <mergeCell ref="C189:C198"/>
-    <mergeCell ref="B139:B148"/>
-    <mergeCell ref="C139:C148"/>
-    <mergeCell ref="B149:B158"/>
-    <mergeCell ref="C149:C158"/>
-    <mergeCell ref="B159:B168"/>
-    <mergeCell ref="C159:C168"/>
-    <mergeCell ref="B109:B118"/>
-    <mergeCell ref="C109:C118"/>
-    <mergeCell ref="B119:B128"/>
-    <mergeCell ref="C119:C128"/>
-    <mergeCell ref="B129:B138"/>
-    <mergeCell ref="C129:C138"/>
-    <mergeCell ref="B79:B88"/>
-    <mergeCell ref="C79:C88"/>
-    <mergeCell ref="B89:B98"/>
-    <mergeCell ref="C89:C98"/>
-    <mergeCell ref="B99:B108"/>
-    <mergeCell ref="C99:C108"/>
-    <mergeCell ref="B49:B58"/>
-    <mergeCell ref="C49:C58"/>
-    <mergeCell ref="B59:B68"/>
-    <mergeCell ref="C59:C68"/>
-    <mergeCell ref="B69:B78"/>
-    <mergeCell ref="C69:C78"/>
-    <mergeCell ref="B19:B28"/>
-    <mergeCell ref="C19:C28"/>
-    <mergeCell ref="B29:B38"/>
-    <mergeCell ref="C29:C38"/>
-    <mergeCell ref="B39:B48"/>
-    <mergeCell ref="C39:C48"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="B2:C5"/>
     <mergeCell ref="B1:G1"/>
@@ -3725,11 +3740,46 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="C19:C28"/>
+    <mergeCell ref="B29:B38"/>
+    <mergeCell ref="C29:C38"/>
+    <mergeCell ref="B39:B48"/>
+    <mergeCell ref="C39:C48"/>
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="C49:C58"/>
+    <mergeCell ref="B59:B68"/>
+    <mergeCell ref="C59:C68"/>
+    <mergeCell ref="B69:B78"/>
+    <mergeCell ref="C69:C78"/>
+    <mergeCell ref="B79:B88"/>
+    <mergeCell ref="C79:C88"/>
+    <mergeCell ref="B89:B98"/>
+    <mergeCell ref="C89:C98"/>
+    <mergeCell ref="B99:B108"/>
+    <mergeCell ref="C99:C108"/>
+    <mergeCell ref="B109:B118"/>
+    <mergeCell ref="C109:C118"/>
+    <mergeCell ref="B119:B128"/>
+    <mergeCell ref="C119:C128"/>
+    <mergeCell ref="B129:B138"/>
+    <mergeCell ref="C129:C138"/>
+    <mergeCell ref="B139:B148"/>
+    <mergeCell ref="C139:C148"/>
+    <mergeCell ref="B149:B158"/>
+    <mergeCell ref="C149:C158"/>
+    <mergeCell ref="B159:B168"/>
+    <mergeCell ref="C159:C168"/>
+    <mergeCell ref="B199:B208"/>
+    <mergeCell ref="C199:C208"/>
+    <mergeCell ref="B209:B218"/>
+    <mergeCell ref="C209:C218"/>
+    <mergeCell ref="B169:B178"/>
+    <mergeCell ref="C169:C178"/>
+    <mergeCell ref="B179:B188"/>
+    <mergeCell ref="C179:C188"/>
+    <mergeCell ref="B189:B198"/>
+    <mergeCell ref="C189:C198"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Pomodoro2020.xlsx and added JIRA
</commit_message>
<xml_diff>
--- a/Pomodoro2020.xlsx
+++ b/Pomodoro2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\04_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEB8AF6-BD6B-49C7-A937-A780DAE34933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F270CB9E-7744-48EC-A95A-338F02B8E9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="122">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -331,9 +331,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Python</t>
-  </si>
-  <si>
     <t>May</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
     <t>Monthly</t>
   </si>
   <si>
-    <t>Weekly</t>
-  </si>
-  <si>
     <t>Yearly</t>
   </si>
   <si>
@@ -379,27 +373,12 @@
     <t>planner</t>
   </si>
   <si>
-    <t>cucumber 적용</t>
-  </si>
-  <si>
-    <t>refactoring</t>
-  </si>
-  <si>
-    <t>3GPP 규격 리뷰</t>
-  </si>
-  <si>
-    <t>JSON</t>
-  </si>
-  <si>
     <t>HTML/CSS, PC App, Java Script, UML, MCU(RTOS), R, MATLAB</t>
   </si>
   <si>
     <t>PDP Process</t>
   </si>
   <si>
-    <t>Android</t>
-  </si>
-  <si>
     <t>XML,PyQt5, Docker</t>
   </si>
   <si>
@@ -409,9 +388,6 @@
     <t>Innovation</t>
   </si>
   <si>
-    <t>Squish</t>
-  </si>
-  <si>
     <t>squish basic</t>
   </si>
   <si>
@@ -424,9 +400,6 @@
     <t>Agile</t>
   </si>
   <si>
-    <t>JIRA, Bamboo CI/CD, Confluence</t>
-  </si>
-  <si>
     <t>Handling CA5G</t>
   </si>
   <si>
@@ -442,18 +415,12 @@
     <t>daily one hour(piano, reading, etc.)</t>
   </si>
   <si>
-    <t>Git, Jenkins</t>
-  </si>
-  <si>
     <t>GDB</t>
   </si>
   <si>
     <t>Cucumber</t>
   </si>
   <si>
-    <t>C++, 3GPP TM, Cucumber</t>
-  </si>
-  <si>
     <t>CPP</t>
   </si>
   <si>
@@ -467,6 +434,100 @@
   </si>
   <si>
     <t>3GPP TM</t>
+  </si>
+  <si>
+    <t>cucumber scpi</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Python, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C++</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, JSON</t>
+    </r>
+  </si>
+  <si>
+    <t>Android, Linux</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Git, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JIRA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Bamboo CI/CD, Confluence</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cucumber</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Squish, </t>
+    </r>
+  </si>
+  <si>
+    <t>C++, JIRA</t>
+  </si>
+  <si>
+    <t>JIRA</t>
+  </si>
+  <si>
+    <t>Weekly
+(5/18 - 5/22)</t>
+  </si>
+  <si>
+    <t>JIRA study</t>
+  </si>
+  <si>
+    <t>cucumber scpi implementing</t>
+  </si>
+  <si>
+    <t>Cpp study</t>
   </si>
 </sst>
 </file>
@@ -477,7 +538,7 @@
     <numFmt numFmtId="164" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="165" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +615,14 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -732,7 +801,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -945,6 +1014,12 @@
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1389,8 +1464,8 @@
   <dimension ref="B1:G218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="18" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="18" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1406,7 +1481,7 @@
   <sheetData>
     <row r="1" spans="2:7">
       <c r="B1" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="58"/>
       <c r="D1" s="58"/>
@@ -1416,29 +1491,27 @@
     </row>
     <row r="2" spans="2:7">
       <c r="B2" s="56" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2" s="57"/>
       <c r="D2" s="63" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E2" s="64"/>
       <c r="F2" s="64"/>
-      <c r="G2" s="37" t="s">
-        <v>75</v>
+      <c r="G2" s="71" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="56"/>
       <c r="C3" s="57"/>
       <c r="D3" s="65" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E3" s="66"/>
       <c r="F3" s="66"/>
-      <c r="G3" s="38" t="s">
-        <v>115</v>
-      </c>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="56"/>
@@ -1447,7 +1520,7 @@
       <c r="E4" s="66"/>
       <c r="F4" s="66"/>
       <c r="G4" s="37" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -1456,34 +1529,34 @@
       <c r="D5" s="65"/>
       <c r="E5" s="66"/>
       <c r="F5" s="66"/>
-      <c r="G5" s="37" t="s">
-        <v>96</v>
+      <c r="G5" s="38" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="56" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="67" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E6" s="68"/>
       <c r="F6" s="68"/>
-      <c r="G6" s="36" t="s">
-        <v>97</v>
+      <c r="G6" s="37" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="56"/>
       <c r="C7" s="57"/>
       <c r="D7" s="67" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E7" s="68"/>
       <c r="F7" s="68"/>
-      <c r="G7" s="36" t="s">
-        <v>112</v>
+      <c r="G7" s="37" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="2:7">
@@ -1493,7 +1566,7 @@
       <c r="E8" s="68"/>
       <c r="F8" s="68"/>
       <c r="G8" s="36" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="2:7">
@@ -1503,93 +1576,91 @@
       <c r="E9" s="68"/>
       <c r="F9" s="68"/>
       <c r="G9" s="36" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="60"/>
       <c r="D10" s="69" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E10" s="70"/>
       <c r="F10" s="70"/>
       <c r="G10" s="36" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="59"/>
       <c r="C11" s="60"/>
       <c r="D11" s="69" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E11" s="70"/>
       <c r="F11" s="70"/>
       <c r="G11" s="36" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="59"/>
       <c r="C12" s="60"/>
       <c r="D12" s="69" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E12" s="70"/>
       <c r="F12" s="70"/>
       <c r="G12" s="36" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="59"/>
       <c r="C13" s="60"/>
-      <c r="D13" s="69" t="s">
-        <v>103</v>
-      </c>
+      <c r="D13" s="69"/>
       <c r="E13" s="70"/>
       <c r="F13" s="70"/>
       <c r="G13" s="36"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="61" t="s">
-        <v>87</v>
+      <c r="B14" s="72" t="s">
+        <v>118</v>
       </c>
       <c r="C14" s="62"/>
       <c r="D14" s="54" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="36" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="61"/>
       <c r="C15" s="62"/>
       <c r="D15" s="54" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="E15" s="55"/>
       <c r="F15" s="55"/>
       <c r="G15" s="36" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="61"/>
       <c r="C16" s="62"/>
       <c r="D16" s="54" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="E16" s="55"/>
       <c r="F16" s="55"/>
       <c r="G16" s="36" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="2:7">
@@ -1671,7 +1742,7 @@
         <v>16</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="20"/>
@@ -1683,7 +1754,7 @@
         <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="6"/>
@@ -1695,7 +1766,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="24"/>
@@ -1707,7 +1778,7 @@
         <v>19</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="6"/>
@@ -1719,7 +1790,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
@@ -1755,7 +1826,7 @@
         <v>14</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F30" s="23"/>
       <c r="G30" s="24"/>
@@ -1767,7 +1838,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F31" s="23"/>
       <c r="G31" s="25"/>
@@ -1796,10 +1867,10 @@
       <c r="B34" s="40"/>
       <c r="C34" s="43"/>
       <c r="D34" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F34" s="21"/>
       <c r="G34" s="24"/>
@@ -1808,10 +1879,10 @@
       <c r="B35" s="40"/>
       <c r="C35" s="43"/>
       <c r="D35" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="24"/>
@@ -1820,10 +1891,10 @@
       <c r="B36" s="40"/>
       <c r="C36" s="43"/>
       <c r="D36" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="24"/>
@@ -1832,10 +1903,10 @@
       <c r="B37" s="40"/>
       <c r="C37" s="43"/>
       <c r="D37" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F37" s="23"/>
       <c r="G37" s="24"/>
@@ -1871,10 +1942,10 @@
         <v>14</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G40" s="24"/>
     </row>
@@ -1885,10 +1956,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G41" s="24"/>
     </row>
@@ -1909,7 +1980,7 @@
         <v>16</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="20"/>
@@ -1921,10 +1992,10 @@
         <v>17</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -1935,10 +2006,10 @@
         <v>18</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G45" s="24"/>
     </row>
@@ -1949,7 +2020,7 @@
         <v>19</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="6"/>
@@ -1961,10 +2032,10 @@
         <v>20</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G47" s="24"/>
     </row>
@@ -1999,10 +2070,10 @@
         <v>14</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G50" s="24"/>
     </row>
@@ -2013,10 +2084,10 @@
         <v>15</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G51" s="25"/>
     </row>
@@ -2044,33 +2115,39 @@
       <c r="B54" s="52"/>
       <c r="C54" s="43"/>
       <c r="D54" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F54" s="21"/>
+        <v>109</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>107</v>
+      </c>
       <c r="G54" s="24"/>
     </row>
     <row r="55" spans="2:7">
       <c r="B55" s="52"/>
       <c r="C55" s="43"/>
       <c r="D55" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F55" s="23"/>
+        <v>109</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>107</v>
+      </c>
       <c r="G55" s="24"/>
     </row>
     <row r="56" spans="2:7">
       <c r="B56" s="52"/>
       <c r="C56" s="43"/>
       <c r="D56" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" s="22"/>
+        <v>83</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>105</v>
+      </c>
       <c r="F56" s="21"/>
       <c r="G56" s="24"/>
     </row>
@@ -2078,9 +2155,11 @@
       <c r="B57" s="52"/>
       <c r="C57" s="43"/>
       <c r="D57" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E57" s="22"/>
+        <v>84</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>105</v>
+      </c>
       <c r="F57" s="23"/>
       <c r="G57" s="24"/>
     </row>
@@ -2114,7 +2193,9 @@
       <c r="D60" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E60" s="22"/>
+      <c r="E60" s="22" t="s">
+        <v>110</v>
+      </c>
       <c r="F60" s="23"/>
       <c r="G60" s="24"/>
     </row>
@@ -2124,7 +2205,9 @@
       <c r="D61" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E61" s="22"/>
+      <c r="E61" s="22" t="s">
+        <v>110</v>
+      </c>
       <c r="F61" s="23"/>
       <c r="G61" s="24"/>
     </row>
@@ -2144,7 +2227,9 @@
       <c r="D63" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E63" s="3"/>
+      <c r="E63" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="F63" s="7"/>
       <c r="G63" s="20"/>
     </row>
@@ -2154,7 +2239,9 @@
       <c r="D64" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="F64" s="2"/>
       <c r="G64" s="6"/>
     </row>
@@ -2164,7 +2251,9 @@
       <c r="D65" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E65" s="22"/>
+      <c r="E65" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="F65" s="21"/>
       <c r="G65" s="24"/>
     </row>
@@ -2174,7 +2263,9 @@
       <c r="D66" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="F66" s="2"/>
       <c r="G66" s="6"/>
     </row>
@@ -2184,7 +2275,9 @@
       <c r="D67" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E67" s="22"/>
+      <c r="E67" s="22" t="s">
+        <v>105</v>
+      </c>
       <c r="F67" s="23"/>
       <c r="G67" s="24"/>
     </row>
@@ -2360,7 +2453,7 @@
       <c r="B84" s="40"/>
       <c r="C84" s="43"/>
       <c r="D84" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E84" s="22"/>
       <c r="F84" s="21"/>
@@ -2370,7 +2463,7 @@
       <c r="B85" s="40"/>
       <c r="C85" s="43"/>
       <c r="D85" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E85" s="22"/>
       <c r="F85" s="23"/>
@@ -2380,7 +2473,7 @@
       <c r="B86" s="40"/>
       <c r="C86" s="43"/>
       <c r="D86" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E86" s="22"/>
       <c r="F86" s="21"/>
@@ -2390,7 +2483,7 @@
       <c r="B87" s="40"/>
       <c r="C87" s="43"/>
       <c r="D87" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E87" s="22"/>
       <c r="F87" s="23"/>
@@ -2568,7 +2661,7 @@
       <c r="B104" s="40"/>
       <c r="C104" s="43"/>
       <c r="D104" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E104" s="22"/>
       <c r="F104" s="21"/>
@@ -2578,7 +2671,7 @@
       <c r="B105" s="40"/>
       <c r="C105" s="43"/>
       <c r="D105" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E105" s="22"/>
       <c r="F105" s="23"/>
@@ -2588,7 +2681,7 @@
       <c r="B106" s="40"/>
       <c r="C106" s="43"/>
       <c r="D106" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E106" s="22"/>
       <c r="F106" s="21"/>
@@ -2598,7 +2691,7 @@
       <c r="B107" s="40"/>
       <c r="C107" s="43"/>
       <c r="D107" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E107" s="22"/>
       <c r="F107" s="23"/>
@@ -2880,7 +2973,7 @@
       <c r="B134" s="40"/>
       <c r="C134" s="43"/>
       <c r="D134" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E134" s="22"/>
       <c r="F134" s="21"/>
@@ -2890,7 +2983,7 @@
       <c r="B135" s="40"/>
       <c r="C135" s="43"/>
       <c r="D135" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E135" s="22"/>
       <c r="F135" s="23"/>
@@ -2900,7 +2993,7 @@
       <c r="B136" s="40"/>
       <c r="C136" s="43"/>
       <c r="D136" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E136" s="22"/>
       <c r="F136" s="21"/>
@@ -2910,7 +3003,7 @@
       <c r="B137" s="40"/>
       <c r="C137" s="43"/>
       <c r="D137" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E137" s="22"/>
       <c r="F137" s="23"/>
@@ -3088,7 +3181,7 @@
       <c r="B154" s="40"/>
       <c r="C154" s="43"/>
       <c r="D154" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E154" s="22"/>
       <c r="F154" s="21"/>
@@ -3098,7 +3191,7 @@
       <c r="B155" s="40"/>
       <c r="C155" s="43"/>
       <c r="D155" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E155" s="22"/>
       <c r="F155" s="23"/>
@@ -3108,7 +3201,7 @@
       <c r="B156" s="40"/>
       <c r="C156" s="43"/>
       <c r="D156" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E156" s="22"/>
       <c r="F156" s="21"/>
@@ -3118,7 +3211,7 @@
       <c r="B157" s="40"/>
       <c r="C157" s="43"/>
       <c r="D157" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E157" s="22"/>
       <c r="F157" s="23"/>
@@ -3241,7 +3334,7 @@
     <row r="169" spans="2:7">
       <c r="B169" s="45"/>
       <c r="C169" s="48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>13</v>
@@ -3343,7 +3436,7 @@
     <row r="179" spans="2:7">
       <c r="B179" s="39"/>
       <c r="C179" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D179" s="21" t="s">
         <v>13</v>
@@ -3396,7 +3489,7 @@
       <c r="B184" s="40"/>
       <c r="C184" s="43"/>
       <c r="D184" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E184" s="22"/>
       <c r="F184" s="21"/>
@@ -3406,7 +3499,7 @@
       <c r="B185" s="40"/>
       <c r="C185" s="43"/>
       <c r="D185" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E185" s="22"/>
       <c r="F185" s="23"/>
@@ -3416,7 +3509,7 @@
       <c r="B186" s="40"/>
       <c r="C186" s="43"/>
       <c r="D186" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E186" s="22"/>
       <c r="F186" s="21"/>
@@ -3426,7 +3519,7 @@
       <c r="B187" s="40"/>
       <c r="C187" s="43"/>
       <c r="D187" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E187" s="22"/>
       <c r="F187" s="23"/>
@@ -3445,7 +3538,7 @@
     <row r="189" spans="2:7">
       <c r="B189" s="45"/>
       <c r="C189" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>13</v>
@@ -3547,7 +3640,7 @@
     <row r="199" spans="2:7">
       <c r="B199" s="39"/>
       <c r="C199" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D199" s="21" t="s">
         <v>13</v>
@@ -3600,7 +3693,7 @@
       <c r="B204" s="40"/>
       <c r="C204" s="43"/>
       <c r="D204" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E204" s="22"/>
       <c r="F204" s="21"/>
@@ -3610,7 +3703,7 @@
       <c r="B205" s="40"/>
       <c r="C205" s="43"/>
       <c r="D205" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E205" s="22"/>
       <c r="F205" s="23"/>
@@ -3620,7 +3713,7 @@
       <c r="B206" s="40"/>
       <c r="C206" s="43"/>
       <c r="D206" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E206" s="22"/>
       <c r="F206" s="21"/>
@@ -3630,7 +3723,7 @@
       <c r="B207" s="40"/>
       <c r="C207" s="43"/>
       <c r="D207" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E207" s="22"/>
       <c r="F207" s="23"/>
@@ -3649,7 +3742,7 @@
     <row r="209" spans="2:7">
       <c r="B209" s="39"/>
       <c r="C209" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>13</v>

</xml_diff>